<commit_message>
update plots congreso masi
</commit_message>
<xml_diff>
--- a/data/analisis_estadistico.xlsx
+++ b/data/analisis_estadistico.xlsx
@@ -7744,7 +7744,7 @@
         <v>63</v>
       </c>
       <c r="C24" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -7991,7 +7991,7 @@
         <v>63</v>
       </c>
       <c r="C25" t="n">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -8238,7 +8238,7 @@
         <v>65</v>
       </c>
       <c r="C26" t="n">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -8485,7 +8485,7 @@
         <v>71</v>
       </c>
       <c r="C27" t="n">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -8732,7 +8732,7 @@
         <v>71</v>
       </c>
       <c r="C28" t="n">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -8979,7 +8979,7 @@
         <v>74</v>
       </c>
       <c r="C29" t="n">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -9226,7 +9226,7 @@
         <v>74</v>
       </c>
       <c r="C30" t="n">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -9473,7 +9473,7 @@
         <v>74</v>
       </c>
       <c r="C31" t="n">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -9720,7 +9720,7 @@
         <v>74</v>
       </c>
       <c r="C32" t="n">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -9967,7 +9967,7 @@
         <v>74</v>
       </c>
       <c r="C33" t="n">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -10214,7 +10214,7 @@
         <v>74</v>
       </c>
       <c r="C34" t="n">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -10461,7 +10461,7 @@
         <v>74</v>
       </c>
       <c r="C35" t="n">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -10708,7 +10708,7 @@
         <v>74</v>
       </c>
       <c r="C36" t="n">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -10955,7 +10955,7 @@
         <v>76</v>
       </c>
       <c r="C37" t="n">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -11202,7 +11202,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="n">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -11449,7 +11449,7 @@
         <v>82</v>
       </c>
       <c r="C39" t="n">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -11696,7 +11696,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="n">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -11943,7 +11943,7 @@
         <v>86</v>
       </c>
       <c r="C41" t="n">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -12194,7 +12194,7 @@
         <v>86</v>
       </c>
       <c r="C42" t="n">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -12445,7 +12445,7 @@
         <v>91</v>
       </c>
       <c r="C43" t="n">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -12692,7 +12692,7 @@
         <v>91</v>
       </c>
       <c r="C44" t="n">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -12941,7 +12941,7 @@
         <v>91</v>
       </c>
       <c r="C45" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -13190,7 +13190,7 @@
         <v>91</v>
       </c>
       <c r="C46" t="n">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -13437,7 +13437,7 @@
         <v>91</v>
       </c>
       <c r="C47" t="n">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -13686,7 +13686,7 @@
         <v>91</v>
       </c>
       <c r="C48" t="n">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -13935,7 +13935,7 @@
         <v>94</v>
       </c>
       <c r="C49" t="n">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -14184,7 +14184,7 @@
         <v>94</v>
       </c>
       <c r="C50" t="n">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -14433,7 +14433,7 @@
         <v>95</v>
       </c>
       <c r="C51" t="n">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -14680,7 +14680,7 @@
         <v>95</v>
       </c>
       <c r="C52" t="n">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -14927,7 +14927,7 @@
         <v>95</v>
       </c>
       <c r="C53" t="n">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -15174,7 +15174,7 @@
         <v>95</v>
       </c>
       <c r="C54" t="n">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -15421,7 +15421,7 @@
         <v>95</v>
       </c>
       <c r="C55" t="n">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -15668,7 +15668,7 @@
         <v>95</v>
       </c>
       <c r="C56" t="n">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -15915,7 +15915,7 @@
         <v>95</v>
       </c>
       <c r="C57" t="n">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -16162,7 +16162,7 @@
         <v>95</v>
       </c>
       <c r="C58" t="n">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -16409,7 +16409,7 @@
         <v>95</v>
       </c>
       <c r="C59" t="n">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -16656,7 +16656,7 @@
         <v>95</v>
       </c>
       <c r="C60" t="n">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -16903,7 +16903,7 @@
         <v>96</v>
       </c>
       <c r="C61" t="n">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -17158,7 +17158,7 @@
         <v>98</v>
       </c>
       <c r="C62" t="n">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -17405,7 +17405,7 @@
         <v>98</v>
       </c>
       <c r="C63" t="n">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -17652,7 +17652,7 @@
         <v>98</v>
       </c>
       <c r="C64" t="n">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -17899,7 +17899,7 @@
         <v>98</v>
       </c>
       <c r="C65" t="n">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>

</xml_diff>